<commit_message>
Se cargo la base de datos de información de AUTOGENERACION
</commit_message>
<xml_diff>
--- a/DataBases/BI - Soporte Declaración de Producción GLP 2022-2026.xlsx
+++ b/DataBases/BI - Soporte Declaración de Producción GLP 2022-2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40589E8-63D7-4038-82D2-60F41593FB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D77BC09-9E17-4AE8-89F3-16F4A8952616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="4350" windowWidth="21600" windowHeight="11430" tabRatio="884" firstSheet="5" activeTab="8" xr2:uid="{C73C23FF-6F55-4CFC-A14F-DE8893533A35}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" firstSheet="5" activeTab="9" xr2:uid="{C73C23FF-6F55-4CFC-A14F-DE8893533A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Dina-19" sheetId="34" r:id="rId1"/>
@@ -385,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5397" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5398" uniqueCount="95">
   <si>
     <t>MES</t>
   </si>
@@ -668,6 +668,9 @@
   <si>
     <t>g/m</t>
   </si>
+  <si>
+    <t>PJ</t>
+  </si>
 </sst>
 </file>
 
@@ -790,7 +793,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -828,6 +831,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -837,7 +849,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -934,6 +946,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="3" xr:uid="{847A4165-B349-4759-982C-59EF67651A8B}"/>
@@ -2333,16 +2349,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4906,8 +4922,8 @@
   </sheetPr>
   <dimension ref="D5:AA106"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,6 +5041,10 @@
         <f>BD_Producido!W47</f>
         <v>25.697326407099602</v>
       </c>
+      <c r="O7" s="22">
+        <f>+SUM(G7:K7)</f>
+        <v>15.531263974566265</v>
+      </c>
       <c r="R7">
         <v>2019</v>
       </c>
@@ -5090,6 +5110,10 @@
         <f>BD_Producido!W48</f>
         <v>36.411311851387559</v>
       </c>
+      <c r="O8" s="22">
+        <f t="shared" ref="O8:O14" si="0">+SUM(G8:K8)</f>
+        <v>26.085675133197142</v>
+      </c>
       <c r="R8">
         <v>2020</v>
       </c>
@@ -5155,6 +5179,10 @@
         <f>BD_Producido!W49</f>
         <v>36.498202534791062</v>
       </c>
+      <c r="O9" s="22">
+        <f t="shared" si="0"/>
+        <v>26.243066627795077</v>
+      </c>
       <c r="R9">
         <v>2021</v>
       </c>
@@ -5221,6 +5249,10 @@
         <f>BD_Producido!W50</f>
         <v>37.59601484087726</v>
       </c>
+      <c r="O10" s="22">
+        <f t="shared" si="0"/>
+        <v>25.340490384312478</v>
+      </c>
       <c r="R10">
         <v>2022</v>
       </c>
@@ -5286,6 +5318,10 @@
         <f>BD_Producido!W51</f>
         <v>36.882404585464215</v>
       </c>
+      <c r="O11" s="22">
+        <f t="shared" si="0"/>
+        <v>24.854518792067424</v>
+      </c>
       <c r="R11">
         <v>2023</v>
       </c>
@@ -5351,6 +5387,10 @@
         <f>BD_Producido!W52</f>
         <v>33.982118684569222</v>
       </c>
+      <c r="O12" s="22">
+        <f t="shared" si="0"/>
+        <v>21.754676513806682</v>
+      </c>
       <c r="R12">
         <v>2024</v>
       </c>
@@ -5416,6 +5456,10 @@
         <f>BD_Producido!W53</f>
         <v>29.992352436575903</v>
       </c>
+      <c r="O13" s="22">
+        <f t="shared" si="0"/>
+        <v>17.869716995554704</v>
+      </c>
       <c r="R13">
         <v>2025</v>
       </c>
@@ -5480,6 +5524,10 @@
       <c r="M14" s="22">
         <f>BD_Producido!W54</f>
         <v>28.036453981121859</v>
+      </c>
+      <c r="O14" s="22">
+        <f t="shared" si="0"/>
+        <v>15.702434330820754</v>
       </c>
       <c r="R14">
         <v>2026</v>
@@ -5624,6 +5672,10 @@
         <f>BD_Consumido!W47</f>
         <v>3.9303688536537207</v>
       </c>
+      <c r="O19" s="22">
+        <f>+SUM(G19:K19)</f>
+        <v>2.3052550363759901</v>
+      </c>
       <c r="P19">
         <v>2019</v>
       </c>
@@ -5632,29 +5684,29 @@
         <v>0.15405477025270098</v>
       </c>
       <c r="R19" s="41">
-        <f t="shared" ref="R19:V19" si="0">+F19/F7</f>
+        <f t="shared" ref="R19:V19" si="1">+F19/F7</f>
         <v>0.163130368385425</v>
       </c>
       <c r="S19" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T19" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U19" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.20013123783141776</v>
       </c>
       <c r="V19" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W19" s="41"/>
       <c r="X19" s="41"/>
       <c r="Y19" s="41">
-        <f t="shared" ref="Y19" si="1">+M19/M7</f>
+        <f t="shared" ref="Y19" si="2">+M19/M7</f>
         <v>0.1529485515881468</v>
       </c>
     </row>
@@ -5695,40 +5747,44 @@
         <f>BD_Consumido!W48</f>
         <v>12.532228576701115</v>
       </c>
+      <c r="O20" s="22">
+        <f t="shared" ref="O20:O26" si="3">+SUM(G20:K20)</f>
+        <v>11.222710674860284</v>
+      </c>
       <c r="P20">
         <v>2020</v>
       </c>
       <c r="Q20" s="41">
-        <f t="shared" ref="Q20:Q26" si="2">+E20/E8</f>
+        <f t="shared" ref="Q20:Q26" si="4">+E20/E8</f>
         <v>0.11590771298142388</v>
       </c>
       <c r="R20" s="41">
-        <f t="shared" ref="R20:R26" si="3">+F20/F8</f>
+        <f t="shared" ref="R20:R26" si="5">+F20/F8</f>
         <v>0.13677951758401249</v>
       </c>
       <c r="S20" s="41">
-        <f t="shared" ref="S20:S24" si="4">+G20/G8</f>
+        <f t="shared" ref="S20:S24" si="6">+G20/G8</f>
         <v>0</v>
       </c>
       <c r="T20" s="41">
-        <f t="shared" ref="T20:T26" si="5">+H20/H8</f>
+        <f t="shared" ref="T20:T26" si="7">+H20/H8</f>
         <v>8.2187866631770329E-2</v>
       </c>
       <c r="U20" s="41">
-        <f t="shared" ref="U20:U26" si="6">+I20/I8</f>
+        <f t="shared" ref="U20:U26" si="8">+I20/I8</f>
         <v>0.88546042212861853</v>
       </c>
       <c r="V20" s="41">
-        <f t="shared" ref="V20:V26" si="7">+J20/J8</f>
+        <f t="shared" ref="V20:V26" si="9">+J20/J8</f>
         <v>0</v>
       </c>
       <c r="W20" s="41">
-        <f t="shared" ref="W20:W21" si="8">+K20/K8</f>
+        <f t="shared" ref="W20:W21" si="10">+K20/K8</f>
         <v>0</v>
       </c>
       <c r="X20" s="41"/>
       <c r="Y20" s="41">
-        <f t="shared" ref="Y20:Y26" si="9">+M20/M8</f>
+        <f t="shared" ref="Y20:Y26" si="11">+M20/M8</f>
         <v>0.34418503315264481</v>
       </c>
     </row>
@@ -5769,40 +5825,44 @@
         <f>BD_Consumido!W49</f>
         <v>14.244641324818891</v>
       </c>
+      <c r="O21" s="22">
+        <f t="shared" si="3"/>
+        <v>12.8421668203575</v>
+      </c>
       <c r="P21">
         <v>2021</v>
       </c>
       <c r="Q21" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.14075277089680155</v>
       </c>
       <c r="R21" s="41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.13242258931901149</v>
       </c>
       <c r="S21" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T21" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.11199254112697511</v>
       </c>
       <c r="U21" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="V21" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W21" s="41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="X21" s="41"/>
       <c r="Y21" s="41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.3902833656326094</v>
       </c>
     </row>
@@ -5844,37 +5904,41 @@
         <f>BD_Consumido!W50</f>
         <v>7.8833962630340109</v>
       </c>
+      <c r="O22" s="22">
+        <f t="shared" si="3"/>
+        <v>4.9725616592787869</v>
+      </c>
       <c r="P22">
         <v>2022</v>
       </c>
       <c r="Q22" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.12152481352242414</v>
       </c>
       <c r="R22" s="41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.31368170130091172</v>
       </c>
       <c r="S22" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="T22" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.2943751298862089E-2</v>
       </c>
       <c r="U22" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.28868562382529195</v>
       </c>
       <c r="V22" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W22" s="41"/>
       <c r="X22" s="41"/>
       <c r="Y22" s="41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.20968701859492248</v>
       </c>
     </row>
@@ -5915,37 +5979,41 @@
         <f>BD_Consumido!W51</f>
         <v>8.3970894010535595</v>
       </c>
+      <c r="O23" s="22">
+        <f t="shared" si="3"/>
+        <v>5.3043326997274622</v>
+      </c>
       <c r="P23">
         <v>2023</v>
       </c>
       <c r="Q23" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.126984126984127</v>
       </c>
       <c r="R23" s="41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.35375218502079925</v>
       </c>
       <c r="S23" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="T23" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U23" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.4231899460823732</v>
       </c>
       <c r="V23" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W23" s="41"/>
       <c r="X23" s="41"/>
       <c r="Y23" s="41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.2276719616150773</v>
       </c>
     </row>
@@ -5986,37 +6054,41 @@
         <f>BD_Consumido!W52</f>
         <v>8.4007930264185156</v>
       </c>
+      <c r="O24" s="22">
+        <f t="shared" si="3"/>
+        <v>5.2995630190613872</v>
+      </c>
       <c r="P24">
         <v>2024</v>
       </c>
       <c r="Q24" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.12698412698412698</v>
       </c>
       <c r="R24" s="41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.3454379894036303</v>
       </c>
       <c r="S24" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="T24" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U24" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.53901258557495457</v>
       </c>
       <c r="V24" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W24" s="41"/>
       <c r="X24" s="41"/>
       <c r="Y24" s="41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.24721216191364759</v>
       </c>
     </row>
@@ -6057,104 +6129,143 @@
         <f>BD_Consumido!W53</f>
         <v>8.0438238490702112</v>
       </c>
+      <c r="O25" s="22">
+        <f t="shared" si="3"/>
+        <v>4.9510671477441139</v>
+      </c>
       <c r="P25">
         <v>2025</v>
       </c>
       <c r="Q25" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.12881626914429631</v>
       </c>
       <c r="R25" s="41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.34536516079758606</v>
       </c>
       <c r="S25" s="41"/>
       <c r="T25" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U25" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.66023144187037919</v>
       </c>
       <c r="V25" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W25" s="41"/>
       <c r="X25" s="41"/>
       <c r="Y25" s="41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.2681958297896202</v>
       </c>
     </row>
     <row r="26" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D26">
+      <c r="D26" s="46">
         <f>BD_Consumido!N54</f>
         <v>2026</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="47">
         <f>BD_Consumido!O54</f>
         <v>0.65076446599449611</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="47">
         <f>BD_Consumido!P54</f>
         <v>2.4419922353316008</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="47">
         <f>BD_Consumido!Q54</f>
         <v>0</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="47">
         <f>BD_Consumido!R54</f>
         <v>0</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="47">
         <f>BD_Consumido!S54</f>
         <v>4.9510671477441139</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J26" s="47">
         <f>BD_Consumido!T54</f>
         <v>0</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="47">
         <f>BD_Consumido!U54</f>
         <v>0</v>
       </c>
-      <c r="M26" s="22">
+      <c r="L26" s="46"/>
+      <c r="M26" s="47">
         <f>BD_Consumido!W54</f>
         <v>8.0438238490702112</v>
       </c>
+      <c r="O26" s="22">
+        <f t="shared" si="3"/>
+        <v>4.9510671477441139</v>
+      </c>
       <c r="P26">
         <v>2026</v>
       </c>
       <c r="Q26" s="41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.126984126984127</v>
       </c>
       <c r="R26" s="41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.33873043815515769</v>
       </c>
       <c r="S26" s="41"/>
       <c r="T26" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U26" s="41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.73346577560228654</v>
       </c>
       <c r="V26" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W26" s="41"/>
       <c r="X26" s="41"/>
       <c r="Y26" s="41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.28690589239589503</v>
       </c>
+    </row>
+    <row r="27" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="G27" s="22">
+        <f>+AVERAGE(G19:G26)</f>
+        <v>0.18690003129516447</v>
+      </c>
+      <c r="H27" s="22">
+        <f>+AVERAGE(H19:H26)</f>
+        <v>0.38547789794507747</v>
+      </c>
+      <c r="I27" s="22">
+        <f>+AVERAGE(I22:I26)</f>
+        <v>4.6132154986544478</v>
+      </c>
+      <c r="J27" s="22">
+        <f t="shared" ref="H27:M27" si="12">+AVERAGE(J19:J26)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22">
+        <f>+AVERAGE(M20:M26)</f>
+        <v>9.649399470023786</v>
+      </c>
+    </row>
+    <row r="28" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="H28" s="22"/>
     </row>
     <row r="30" spans="4:25" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E30" s="44" t="s">
@@ -6202,295 +6313,350 @@
         <v>3.1020321301919696</v>
       </c>
       <c r="F32" s="22">
-        <f t="shared" ref="F32:K32" si="10">+F7-F19</f>
+        <f t="shared" ref="F32:K32" si="13">+F7-F19</f>
         <v>5.4389164850636416</v>
       </c>
       <c r="G32" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.72587988512140356</v>
       </c>
       <c r="H32" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.0516035471805942</v>
       </c>
       <c r="I32" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>9.2134616884855305</v>
       </c>
       <c r="J32" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.23506381740274676</v>
       </c>
       <c r="K32" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M32" s="22">
         <f>+M7-M19</f>
         <v>21.766957553445881</v>
       </c>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O32" s="22"/>
+    </row>
+    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>2020</v>
       </c>
       <c r="E33" s="22">
-        <f t="shared" ref="E33:K33" si="11">+E8-E20</f>
+        <f t="shared" ref="E33:K33" si="14">+E8-E20</f>
         <v>4.3551740567638122</v>
       </c>
       <c r="F33" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>4.6609447595857718</v>
       </c>
       <c r="G33" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.53702859618588517</v>
       </c>
       <c r="H33" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>10.315774102933412</v>
       </c>
       <c r="I33" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.3322315325968006</v>
       </c>
       <c r="J33" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.25599010194730198</v>
       </c>
       <c r="K33" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>2.4219401246734575</v>
       </c>
       <c r="M33" s="22">
-        <f t="shared" ref="M33:M39" si="12">+M8-M20</f>
+        <f t="shared" ref="M33:M39" si="15">+M8-M20</f>
         <v>23.879083274686444</v>
       </c>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+    </row>
+    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>2021</v>
       </c>
       <c r="E34" s="22">
-        <f t="shared" ref="E34:K34" si="13">+E9-E21</f>
+        <f t="shared" ref="E34:K34" si="16">+E9-E21</f>
         <v>4.5862846568327074</v>
       </c>
       <c r="F34" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>4.2663767457018862</v>
       </c>
       <c r="G34" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.4127774497680638</v>
       </c>
       <c r="H34" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>9.8540228588051431</v>
       </c>
       <c r="I34" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J34" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.24518398775720535</v>
       </c>
       <c r="K34" s="22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>2.888915511107164</v>
       </c>
       <c r="M34" s="22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>22.253561209972169</v>
       </c>
-    </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O34" s="22"/>
+      <c r="Q34" s="48"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="48"/>
+    </row>
+    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>2022</v>
       </c>
       <c r="E35" s="22">
-        <f t="shared" ref="E35:K35" si="14">+E10-E22</f>
+        <f t="shared" ref="E35:K35" si="17">+E10-E22</f>
         <v>4.2676370151614096</v>
       </c>
       <c r="F35" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>5.0770528376481527</v>
       </c>
       <c r="G35" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H35" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>11.658320220889701</v>
       </c>
       <c r="I35" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>8.4738225229325916</v>
       </c>
       <c r="J35" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.23578598121139627</v>
       </c>
       <c r="K35" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L35" s="22"/>
       <c r="M35" s="22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>29.712618577843248</v>
       </c>
-    </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O35" s="22"/>
+      <c r="Q35" s="48"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="49"/>
+      <c r="U35" s="48"/>
+    </row>
+    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>2023</v>
       </c>
       <c r="E36" s="22">
-        <f t="shared" ref="E36:K36" si="15">+E11-E23</f>
+        <f t="shared" ref="E36:K36" si="18">+E11-E23</f>
         <v>4.4740057037121606</v>
       </c>
       <c r="F36" s="22">
+        <f t="shared" si="18"/>
+        <v>4.46112338835853</v>
+      </c>
+      <c r="G36" s="22">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="22">
+        <f t="shared" si="18"/>
+        <v>12.750234521122225</v>
+      </c>
+      <c r="I36" s="22">
+        <f t="shared" si="18"/>
+        <v>6.5801627167822385</v>
+      </c>
+      <c r="J36" s="22">
+        <f t="shared" si="18"/>
+        <v>0.21978885443549936</v>
+      </c>
+      <c r="K36" s="22">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="22">
         <f t="shared" si="15"/>
-        <v>4.46112338835853</v>
-      </c>
-      <c r="G36" s="22">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="22">
-        <f t="shared" si="15"/>
-        <v>12.750234521122225</v>
-      </c>
-      <c r="I36" s="22">
-        <f t="shared" si="15"/>
-        <v>6.5801627167822385</v>
-      </c>
-      <c r="J36" s="22">
-        <f t="shared" si="15"/>
-        <v>0.21978885443549936</v>
-      </c>
-      <c r="K36" s="22">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="22">
-        <f t="shared" si="12"/>
         <v>28.485315184410656</v>
       </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O36" s="22"/>
+      <c r="Q36" s="48"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="49"/>
+      <c r="U36" s="48"/>
+    </row>
+    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>2024</v>
       </c>
       <c r="E37" s="22">
-        <f t="shared" ref="E37:K37" si="16">+E12-E24</f>
+        <f t="shared" ref="E37:K37" si="19">+E12-E24</f>
         <v>4.4862632535853448</v>
       </c>
       <c r="F37" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.6399489098200739</v>
       </c>
       <c r="G37" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H37" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>12.067505504975106</v>
       </c>
       <c r="I37" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>4.1882768849079328</v>
       </c>
       <c r="J37" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.19933110486225489</v>
       </c>
       <c r="K37" s="22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="M37" s="22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>25.581325658150707</v>
       </c>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O37" s="22"/>
+      <c r="Q37" s="48"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="48"/>
+    </row>
+    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>2025</v>
       </c>
       <c r="E38" s="22">
-        <f t="shared" ref="E38:K38" si="17">+E13-E25</f>
+        <f t="shared" ref="E38:K38" si="20">+E13-E25</f>
         <v>4.4011165605047911</v>
       </c>
       <c r="F38" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>4.6287621791903089</v>
       </c>
       <c r="G38" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H38" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>10.193808930454354</v>
       </c>
       <c r="I38" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>2.5479200766724697</v>
       </c>
       <c r="J38" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.17692084068376571</v>
       </c>
       <c r="K38" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M38" s="22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>21.948528587505692</v>
       </c>
-    </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O38" s="22"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="49"/>
+      <c r="U38" s="48"/>
+    </row>
+    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>2026</v>
       </c>
       <c r="E39" s="22">
-        <f t="shared" ref="E39:K39" si="18">+E14-E26</f>
+        <f t="shared" ref="E39:K39" si="21">+E14-E26</f>
         <v>4.4740057037121606</v>
       </c>
       <c r="F39" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>4.767257245262849</v>
       </c>
       <c r="G39" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="H39" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>8.7930167117138982</v>
       </c>
       <c r="I39" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.7991689402022359</v>
       </c>
       <c r="J39" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.15918153116050621</v>
       </c>
       <c r="K39" s="22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M39" s="22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>19.992630132051648</v>
       </c>
-    </row>
-    <row r="42" spans="4:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="O39" s="22"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="49"/>
+      <c r="U39" s="48"/>
+    </row>
+    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="Q40" s="48"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="49"/>
+      <c r="U40" s="48"/>
+    </row>
+    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="Q41" s="48"/>
+      <c r="R41" s="48"/>
+      <c r="S41" s="48"/>
+      <c r="T41" s="48"/>
+      <c r="U41" s="48"/>
+    </row>
+    <row r="42" spans="4:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E42" s="44" t="s">
         <v>88</v>
       </c>
@@ -6500,8 +6666,13 @@
       <c r="I42" s="44"/>
       <c r="J42" s="44"/>
       <c r="K42" s="44"/>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="Q42" s="48"/>
+      <c r="R42" s="48"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="48"/>
+      <c r="U42" s="48"/>
+    </row>
+    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>58</v>
       </c>
@@ -6526,8 +6697,13 @@
       <c r="M43" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="48"/>
+      <c r="U43" s="48"/>
+    </row>
+    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E44" s="22" t="s">
         <v>58</v>
       </c>
@@ -6552,8 +6728,13 @@
       <c r="M44" s="22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="Q44" s="48"/>
+      <c r="R44" s="48"/>
+      <c r="S44" s="48"/>
+      <c r="T44" s="48"/>
+      <c r="U44" s="48"/>
+    </row>
+    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>2019</v>
       </c>
@@ -6581,8 +6762,12 @@
       <c r="M45" s="22">
         <v>21.766957553445881</v>
       </c>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="O45" s="22">
+        <f>+AVERAGE(E45:K45)</f>
+        <v>3.1095653647779833</v>
+      </c>
+    </row>
+    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>2020</v>
       </c>
@@ -6611,7 +6796,7 @@
         <v>23.879083274686444</v>
       </c>
     </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D47">
         <v>2021</v>
       </c>
@@ -6641,7 +6826,7 @@
         <v>22.253561209972169</v>
       </c>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D48">
         <v>2022</v>
       </c>
@@ -6784,6 +6969,15 @@
       </c>
       <c r="M52">
         <v>19.992630132051648</v>
+      </c>
+    </row>
+    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G55" s="22">
+        <f>+AVERAGE(G45:J45)</f>
+        <v>3.306502234547569</v>
+      </c>
+      <c r="H55" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="5:15" ht="23.25" x14ac:dyDescent="0.35">
@@ -25955,7 +26149,7 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="A2:J7"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27932,8 +28126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474A44AF-46D5-40CD-894E-02E73C92F2B1}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32:H61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67570,8 +67764,8 @@
   </sheetPr>
   <dimension ref="C3:AY103"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AR1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5:AY15"/>
+    <sheetView showGridLines="0" topLeftCell="I28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W48" sqref="W48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70705,7 +70899,7 @@
         <v>0</v>
       </c>
       <c r="W47" s="22">
-        <f t="shared" ref="W47:W49" si="31">+SUM(O47:U47)</f>
+        <f>+SUM(O47:U47)</f>
         <v>25.697326407099602</v>
       </c>
     </row>
@@ -70773,7 +70967,7 @@
         <v>2.4219401246734575</v>
       </c>
       <c r="W48" s="22">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="W47:W49" si="31">+SUM(O48:U48)</f>
         <v>36.411311851387559</v>
       </c>
     </row>
@@ -72797,7 +72991,7 @@
   </sheetPr>
   <dimension ref="C3:AP103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AH7" sqref="AH7:AN14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Avance en refineria 1: se hizo de nuevo
</commit_message>
<xml_diff>
--- a/DataBases/BI - Soporte Declaración de Producción GLP 2022-2026.xlsx
+++ b/DataBases/BI - Soporte Declaración de Producción GLP 2022-2026.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D77BC09-9E17-4AE8-89F3-16F4A8952616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66246354-E41E-435C-B322-D4D6472BAB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" firstSheet="5" activeTab="9" xr2:uid="{C73C23FF-6F55-4CFC-A14F-DE8893533A35}"/>
   </bookViews>
@@ -849,7 +849,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -940,16 +940,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="3" xr:uid="{847A4165-B349-4759-982C-59EF67651A8B}"/>
@@ -4922,8 +4921,8 @@
   </sheetPr>
   <dimension ref="D5:AA106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,15 +4932,15 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:27" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
       <c r="S5" t="s">
         <v>86</v>
       </c>
@@ -5558,24 +5557,24 @@
       </c>
     </row>
     <row r="17" spans="4:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="P17" s="44" t="s">
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="P17" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="44"/>
-      <c r="V17" s="44"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="46"/>
     </row>
     <row r="18" spans="4:25" x14ac:dyDescent="0.25">
       <c r="E18" t="str">
@@ -6165,40 +6164,40 @@
       </c>
     </row>
     <row r="26" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D26" s="46">
+      <c r="D26" s="44">
         <f>BD_Consumido!N54</f>
         <v>2026</v>
       </c>
-      <c r="E26" s="47">
+      <c r="E26" s="45">
         <f>BD_Consumido!O54</f>
         <v>0.65076446599449611</v>
       </c>
-      <c r="F26" s="47">
+      <c r="F26" s="45">
         <f>BD_Consumido!P54</f>
         <v>2.4419922353316008</v>
       </c>
-      <c r="G26" s="47">
+      <c r="G26" s="45">
         <f>BD_Consumido!Q54</f>
         <v>0</v>
       </c>
-      <c r="H26" s="47">
+      <c r="H26" s="45">
         <f>BD_Consumido!R54</f>
         <v>0</v>
       </c>
-      <c r="I26" s="47">
+      <c r="I26" s="45">
         <f>BD_Consumido!S54</f>
         <v>4.9510671477441139</v>
       </c>
-      <c r="J26" s="47">
+      <c r="J26" s="45">
         <f>BD_Consumido!T54</f>
         <v>0</v>
       </c>
-      <c r="K26" s="47">
+      <c r="K26" s="45">
         <f>BD_Consumido!U54</f>
         <v>0</v>
       </c>
-      <c r="L26" s="46"/>
-      <c r="M26" s="47">
+      <c r="L26" s="44"/>
+      <c r="M26" s="45">
         <f>BD_Consumido!W54</f>
         <v>8.0438238490702112</v>
       </c>
@@ -6251,7 +6250,7 @@
         <v>4.6132154986544478</v>
       </c>
       <c r="J27" s="22">
-        <f t="shared" ref="H27:M27" si="12">+AVERAGE(J19:J26)</f>
+        <f t="shared" ref="J27:K27" si="12">+AVERAGE(J19:J26)</f>
         <v>0</v>
       </c>
       <c r="K27" s="22">
@@ -6267,16 +6266,22 @@
     <row r="28" spans="4:25" x14ac:dyDescent="0.25">
       <c r="H28" s="22"/>
     </row>
+    <row r="29" spans="4:25" x14ac:dyDescent="0.25">
+      <c r="Q29" s="48">
+        <f>+AVERAGE(Q19:Q26)</f>
+        <v>0.13025108971875349</v>
+      </c>
+    </row>
     <row r="30" spans="4:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
     </row>
     <row r="31" spans="4:25" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
@@ -6342,7 +6347,7 @@
       </c>
       <c r="O32" s="22"/>
     </row>
-    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>2020</v>
       </c>
@@ -6383,7 +6388,7 @@
       <c r="S33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>2021</v>
       </c>
@@ -6420,13 +6425,11 @@
         <v>22.253561209972169</v>
       </c>
       <c r="O34" s="22"/>
-      <c r="Q34" s="48"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="49"/>
-      <c r="T34" s="49"/>
-      <c r="U34" s="48"/>
-    </row>
-    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+    </row>
+    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>2022</v>
       </c>
@@ -6464,13 +6467,11 @@
         <v>29.712618577843248</v>
       </c>
       <c r="O35" s="22"/>
-      <c r="Q35" s="48"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="49"/>
-      <c r="U35" s="48"/>
-    </row>
-    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+    </row>
+    <row r="36" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>2023</v>
       </c>
@@ -6507,13 +6508,11 @@
         <v>28.485315184410656</v>
       </c>
       <c r="O36" s="22"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="49"/>
-      <c r="S36" s="49"/>
-      <c r="T36" s="49"/>
-      <c r="U36" s="48"/>
-    </row>
-    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+    </row>
+    <row r="37" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>2024</v>
       </c>
@@ -6550,13 +6549,11 @@
         <v>25.581325658150707</v>
       </c>
       <c r="O37" s="22"/>
-      <c r="Q37" s="48"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="48"/>
-    </row>
-    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+    </row>
+    <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>2025</v>
       </c>
@@ -6593,13 +6590,11 @@
         <v>21.948528587505692</v>
       </c>
       <c r="O38" s="22"/>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="49"/>
-      <c r="S38" s="49"/>
-      <c r="T38" s="49"/>
-      <c r="U38" s="48"/>
-    </row>
-    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+    </row>
+    <row r="39" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>2026</v>
       </c>
@@ -6636,43 +6631,28 @@
         <v>19.992630132051648</v>
       </c>
       <c r="O39" s="22"/>
-      <c r="Q39" s="48"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="49"/>
-      <c r="U39" s="48"/>
-    </row>
-    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="Q40" s="48"/>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
-      <c r="T40" s="49"/>
-      <c r="U40" s="48"/>
-    </row>
-    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="Q41" s="48"/>
-      <c r="R41" s="48"/>
-      <c r="S41" s="48"/>
-      <c r="T41" s="48"/>
-      <c r="U41" s="48"/>
-    </row>
-    <row r="42" spans="4:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E42" s="44" t="s">
+      <c r="R39" s="22"/>
+      <c r="S39" s="22"/>
+      <c r="T39" s="22"/>
+    </row>
+    <row r="40" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
+    </row>
+    <row r="42" spans="4:20" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E42" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
-      <c r="Q42" s="48"/>
-      <c r="R42" s="48"/>
-      <c r="S42" s="49"/>
-      <c r="T42" s="48"/>
-      <c r="U42" s="48"/>
-    </row>
-    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="S42" s="22"/>
+    </row>
+    <row r="43" spans="4:20" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>58</v>
       </c>
@@ -6697,13 +6677,8 @@
       <c r="M43" t="s">
         <v>84</v>
       </c>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="48"/>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
-      <c r="U43" s="48"/>
-    </row>
-    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="4:20" x14ac:dyDescent="0.25">
       <c r="E44" s="22" t="s">
         <v>58</v>
       </c>
@@ -6728,13 +6703,8 @@
       <c r="M44" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="Q44" s="48"/>
-      <c r="R44" s="48"/>
-      <c r="S44" s="48"/>
-      <c r="T44" s="48"/>
-      <c r="U44" s="48"/>
-    </row>
-    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>2019</v>
       </c>
@@ -6767,7 +6737,7 @@
         <v>3.1095653647779833</v>
       </c>
     </row>
-    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>2020</v>
       </c>
@@ -6796,7 +6766,7 @@
         <v>23.879083274686444</v>
       </c>
     </row>
-    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D47">
         <v>2021</v>
       </c>
@@ -6826,7 +6796,7 @@
         <v>22.253561209972169</v>
       </c>
     </row>
-    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D48">
         <v>2022</v>
       </c>
@@ -6981,15 +6951,15 @@
       </c>
     </row>
     <row r="97" spans="5:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F97" s="44" t="s">
+      <c r="F97" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="G97" s="44"/>
-      <c r="H97" s="44"/>
-      <c r="I97" s="44"/>
-      <c r="J97" s="44"/>
-      <c r="K97" s="44"/>
-      <c r="L97" s="44"/>
+      <c r="G97" s="46"/>
+      <c r="H97" s="46"/>
+      <c r="I97" s="46"/>
+      <c r="J97" s="46"/>
+      <c r="K97" s="46"/>
+      <c r="L97" s="46"/>
     </row>
     <row r="98" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
@@ -7293,24 +7263,24 @@
       </c>
     </row>
     <row r="5" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="N5" s="44" t="s">
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="N5" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
@@ -67764,8 +67734,8 @@
   </sheetPr>
   <dimension ref="C3:AY103"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
+    <sheetView showGridLines="0" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67787,51 +67757,51 @@
     </row>
     <row r="5" spans="3:51" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="23"/>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="O5" s="44" t="s">
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="O5" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="Y5" s="44" t="s">
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="Y5" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44"/>
-      <c r="AH5" s="44" t="s">
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="46"/>
+      <c r="AC5" s="46"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AH5" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AI5" s="44"/>
-      <c r="AJ5" s="44"/>
-      <c r="AK5" s="44"/>
-      <c r="AL5" s="44"/>
-      <c r="AM5" s="44"/>
-      <c r="AN5" s="44"/>
-      <c r="AS5" s="44" t="s">
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="46"/>
+      <c r="AL5" s="46"/>
+      <c r="AM5" s="46"/>
+      <c r="AN5" s="46"/>
+      <c r="AS5" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AT5" s="44"/>
-      <c r="AU5" s="44"/>
-      <c r="AV5" s="44"/>
-      <c r="AW5" s="44"/>
-      <c r="AX5" s="44"/>
-      <c r="AY5" s="44"/>
+      <c r="AT5" s="46"/>
+      <c r="AU5" s="46"/>
+      <c r="AV5" s="46"/>
+      <c r="AW5" s="46"/>
+      <c r="AX5" s="46"/>
+      <c r="AY5" s="46"/>
     </row>
     <row r="6" spans="3:51" x14ac:dyDescent="0.25">
       <c r="C6" s="23"/>
@@ -69279,6 +69249,10 @@
         <f>+'Floreña-19'!I12/'Floreña-19'!F12</f>
         <v>0</v>
       </c>
+      <c r="Y16" s="19">
+        <f>+Y7/365</f>
+        <v>2253.928870417391</v>
+      </c>
     </row>
     <row r="17" spans="3:40" x14ac:dyDescent="0.25">
       <c r="C17" s="24">
@@ -69691,6 +69665,10 @@
       <c r="U25" t="s">
         <v>63</v>
       </c>
+      <c r="AH25" s="19">
+        <f>+AVERAGE(AH7:AH14)</f>
+        <v>3014.062358831618</v>
+      </c>
     </row>
     <row r="26" spans="3:40" x14ac:dyDescent="0.25">
       <c r="C26" s="24">
@@ -70081,15 +70059,15 @@
         <f>+'Floreña-19'!I29/'Floreña-19'!F29</f>
         <v>2439948.1993093244</v>
       </c>
-      <c r="O33" s="44" t="s">
+      <c r="O33" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="44"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C34" s="24">
@@ -70768,15 +70746,15 @@
       <c r="J45" s="19">
         <v>0</v>
       </c>
-      <c r="O45" s="44" t="s">
+      <c r="O45" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
-      <c r="T45" s="44"/>
-      <c r="U45" s="44"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="46"/>
+      <c r="T45" s="46"/>
+      <c r="U45" s="46"/>
     </row>
     <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" s="20">
@@ -70967,7 +70945,7 @@
         <v>2.4219401246734575</v>
       </c>
       <c r="W48" s="22">
-        <f t="shared" ref="W47:W49" si="31">+SUM(O48:U48)</f>
+        <f t="shared" ref="W48:W49" si="31">+SUM(O48:U48)</f>
         <v>36.411311851387559</v>
       </c>
     </row>
@@ -72992,7 +72970,7 @@
   <dimension ref="C3:AP103"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH7" sqref="AH7:AN14"/>
+      <selection activeCell="AH19" sqref="AH19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73014,42 +72992,42 @@
     </row>
     <row r="5" spans="3:42" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="23"/>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="O5" s="44" t="s">
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="O5" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="Y5" s="44" t="s">
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="Y5" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44"/>
-      <c r="AH5" s="44" t="s">
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="46"/>
+      <c r="AC5" s="46"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AH5" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="AI5" s="44"/>
-      <c r="AJ5" s="44"/>
-      <c r="AK5" s="44"/>
-      <c r="AL5" s="44"/>
-      <c r="AM5" s="44"/>
-      <c r="AN5" s="44"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="46"/>
+      <c r="AL5" s="46"/>
+      <c r="AM5" s="46"/>
+      <c r="AN5" s="46"/>
     </row>
     <row r="6" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C6" s="23"/>
@@ -74247,7 +74225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C17" s="24">
         <v>43770</v>
       </c>
@@ -74280,7 +74258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C18" s="24">
         <v>43800</v>
       </c>
@@ -74312,8 +74290,12 @@
         <f>+'Floreña-19'!J14/'Floreña-19'!F14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="AH18" s="19">
+        <f>+AVERAGE(AH7:AH14)</f>
+        <v>390.49262932266583</v>
+      </c>
+    </row>
+    <row r="19" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C19" s="24">
         <v>43831</v>
       </c>
@@ -74346,7 +74328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C20" s="24">
         <v>43862</v>
       </c>
@@ -74379,7 +74361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C21" s="24">
         <v>43891</v>
       </c>
@@ -74412,7 +74394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C22" s="24">
         <v>43922</v>
       </c>
@@ -74445,7 +74427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C23" s="24">
         <v>43952</v>
       </c>
@@ -74478,7 +74460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C24" s="24">
         <v>43983</v>
       </c>
@@ -74514,7 +74496,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C25" s="24">
         <v>44013</v>
       </c>
@@ -74568,7 +74550,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C26" s="24">
         <v>44044</v>
       </c>
@@ -74632,7 +74614,7 @@
         <v>95312</v>
       </c>
     </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C27" s="24">
         <v>44075</v>
       </c>
@@ -74695,7 +74677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C28" s="24">
         <v>44105</v>
       </c>
@@ -74731,7 +74713,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C29" s="24">
         <v>44136</v>
       </c>
@@ -74795,7 +74777,7 @@
         <v>9.5311999999999998E-5</v>
       </c>
     </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C30" s="24">
         <v>44166</v>
       </c>
@@ -74859,7 +74841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C31" s="24">
         <v>44197</v>
       </c>
@@ -74892,7 +74874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C32" s="24">
         <v>44228</v>
       </c>
@@ -74957,15 +74939,15 @@
         <f>+'Floreña-19'!J29/'Floreña-19'!F29</f>
         <v>0</v>
       </c>
-      <c r="O33" s="44" t="s">
+      <c r="O33" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="44"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C34" s="24">
@@ -75644,15 +75626,15 @@
       <c r="J45" s="40">
         <v>2</v>
       </c>
-      <c r="O45" s="44" t="s">
+      <c r="O45" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
-      <c r="T45" s="44"/>
-      <c r="U45" s="44"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="46"/>
+      <c r="T45" s="46"/>
+      <c r="U45" s="46"/>
     </row>
     <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" s="20">

</xml_diff>

<commit_message>
Putno de Partida para realizar Analisism, revisar PLANTILLA-DIC11 como ultima versión
</commit_message>
<xml_diff>
--- a/DataBases/BI - Soporte Declaración de Producción GLP 2022-2026.xlsx
+++ b/DataBases/BI - Soporte Declaración de Producción GLP 2022-2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66246354-E41E-435C-B322-D4D6472BAB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385734A4-D562-4C29-B3B1-74361AED8AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" firstSheet="5" activeTab="9" xr2:uid="{C73C23FF-6F55-4CFC-A14F-DE8893533A35}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="884" firstSheet="5" activeTab="7" xr2:uid="{C73C23FF-6F55-4CFC-A14F-DE8893533A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Dina-19" sheetId="34" r:id="rId1"/>
@@ -942,13 +942,13 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="3" xr:uid="{847A4165-B349-4759-982C-59EF67651A8B}"/>
@@ -4921,7 +4921,7 @@
   </sheetPr>
   <dimension ref="D5:AA106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
@@ -4932,15 +4932,15 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:27" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
       <c r="S5" t="s">
         <v>86</v>
       </c>
@@ -5557,24 +5557,24 @@
       </c>
     </row>
     <row r="17" spans="4:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="P17" s="46" t="s">
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="P17" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="46"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
     </row>
     <row r="18" spans="4:25" x14ac:dyDescent="0.25">
       <c r="E18" t="str">
@@ -6267,21 +6267,21 @@
       <c r="H28" s="22"/>
     </row>
     <row r="29" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="Q29" s="48">
+      <c r="Q29" s="46">
         <f>+AVERAGE(Q19:Q26)</f>
         <v>0.13025108971875349</v>
       </c>
     </row>
     <row r="30" spans="4:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
     </row>
     <row r="31" spans="4:25" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
@@ -6641,15 +6641,15 @@
       <c r="T40" s="22"/>
     </row>
     <row r="42" spans="4:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E42" s="46" t="s">
+      <c r="E42" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
       <c r="S42" s="22"/>
     </row>
     <row r="43" spans="4:20" x14ac:dyDescent="0.25">
@@ -6951,15 +6951,15 @@
       </c>
     </row>
     <row r="97" spans="5:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F97" s="46" t="s">
+      <c r="F97" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="G97" s="46"/>
-      <c r="H97" s="46"/>
-      <c r="I97" s="46"/>
-      <c r="J97" s="46"/>
-      <c r="K97" s="46"/>
-      <c r="L97" s="46"/>
+      <c r="G97" s="47"/>
+      <c r="H97" s="47"/>
+      <c r="I97" s="47"/>
+      <c r="J97" s="47"/>
+      <c r="K97" s="47"/>
+      <c r="L97" s="47"/>
     </row>
     <row r="98" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
@@ -7263,24 +7263,24 @@
       </c>
     </row>
     <row r="5" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="N5" s="46" t="s">
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="N5" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
@@ -67734,8 +67734,8 @@
   </sheetPr>
   <dimension ref="C3:AY103"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH26" sqref="AH26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7:AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67754,54 +67754,58 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="AI3" s="19">
+        <f>+AVERAGE(AI7:AI14)</f>
+        <v>4029.9152200919875</v>
+      </c>
     </row>
     <row r="5" spans="3:51" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="23"/>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="O5" s="46" t="s">
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="O5" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="Y5" s="46" t="s">
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="Y5" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="46"/>
-      <c r="AH5" s="46" t="s">
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AH5" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="AI5" s="46"/>
-      <c r="AJ5" s="46"/>
-      <c r="AK5" s="46"/>
-      <c r="AL5" s="46"/>
-      <c r="AM5" s="46"/>
-      <c r="AN5" s="46"/>
-      <c r="AS5" s="46" t="s">
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
+      <c r="AS5" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="AT5" s="46"/>
-      <c r="AU5" s="46"/>
-      <c r="AV5" s="46"/>
-      <c r="AW5" s="46"/>
-      <c r="AX5" s="46"/>
-      <c r="AY5" s="46"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="47"/>
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="47"/>
     </row>
     <row r="6" spans="3:51" x14ac:dyDescent="0.25">
       <c r="C6" s="23"/>
@@ -70059,15 +70063,15 @@
         <f>+'Floreña-19'!I29/'Floreña-19'!F29</f>
         <v>2439948.1993093244</v>
       </c>
-      <c r="O33" s="46" t="s">
+      <c r="O33" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="47"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="47"/>
+      <c r="T33" s="47"/>
+      <c r="U33" s="47"/>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C34" s="24">
@@ -70746,15 +70750,15 @@
       <c r="J45" s="19">
         <v>0</v>
       </c>
-      <c r="O45" s="46" t="s">
+      <c r="O45" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="P45" s="46"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="46"/>
-      <c r="S45" s="46"/>
-      <c r="T45" s="46"/>
-      <c r="U45" s="46"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="47"/>
+      <c r="R45" s="47"/>
+      <c r="S45" s="47"/>
+      <c r="T45" s="47"/>
+      <c r="U45" s="47"/>
     </row>
     <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" s="20">
@@ -72969,8 +72973,8 @@
   </sheetPr>
   <dimension ref="C3:AP103"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH19" sqref="AH19"/>
+    <sheetView showGridLines="0" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH18" sqref="AH18:AI18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72992,42 +72996,42 @@
     </row>
     <row r="5" spans="3:42" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="23"/>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="O5" s="46" t="s">
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="O5" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="Y5" s="46" t="s">
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="Y5" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="46"/>
-      <c r="AH5" s="46" t="s">
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AH5" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="AI5" s="46"/>
-      <c r="AJ5" s="46"/>
-      <c r="AK5" s="46"/>
-      <c r="AL5" s="46"/>
-      <c r="AM5" s="46"/>
-      <c r="AN5" s="46"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
     </row>
     <row r="6" spans="3:42" x14ac:dyDescent="0.25">
       <c r="C6" s="23"/>
@@ -74225,7 +74229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C17" s="24">
         <v>43770</v>
       </c>
@@ -74258,7 +74262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C18" s="24">
         <v>43800</v>
       </c>
@@ -74294,8 +74298,12 @@
         <f>+AVERAGE(AH7:AH14)</f>
         <v>390.49262932266583</v>
       </c>
-    </row>
-    <row r="19" spans="3:34" x14ac:dyDescent="0.25">
+      <c r="AI18" s="19">
+        <f>+AVERAGE(AI7:AI14)</f>
+        <v>1116.7930465985244</v>
+      </c>
+    </row>
+    <row r="19" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C19" s="24">
         <v>43831</v>
       </c>
@@ -74328,7 +74336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C20" s="24">
         <v>43862</v>
       </c>
@@ -74361,7 +74369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C21" s="24">
         <v>43891</v>
       </c>
@@ -74394,7 +74402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C22" s="24">
         <v>43922</v>
       </c>
@@ -74427,7 +74435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C23" s="24">
         <v>43952</v>
       </c>
@@ -74460,7 +74468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C24" s="24">
         <v>43983</v>
       </c>
@@ -74496,7 +74504,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C25" s="24">
         <v>44013</v>
       </c>
@@ -74550,7 +74558,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C26" s="24">
         <v>44044</v>
       </c>
@@ -74614,7 +74622,7 @@
         <v>95312</v>
       </c>
     </row>
-    <row r="27" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C27" s="24">
         <v>44075</v>
       </c>
@@ -74677,7 +74685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C28" s="24">
         <v>44105</v>
       </c>
@@ -74713,7 +74721,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C29" s="24">
         <v>44136</v>
       </c>
@@ -74777,7 +74785,7 @@
         <v>9.5311999999999998E-5</v>
       </c>
     </row>
-    <row r="30" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C30" s="24">
         <v>44166</v>
       </c>
@@ -74841,7 +74849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C31" s="24">
         <v>44197</v>
       </c>
@@ -74874,7 +74882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C32" s="24">
         <v>44228</v>
       </c>
@@ -74939,15 +74947,15 @@
         <f>+'Floreña-19'!J29/'Floreña-19'!F29</f>
         <v>0</v>
       </c>
-      <c r="O33" s="46" t="s">
+      <c r="O33" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="47"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="47"/>
+      <c r="T33" s="47"/>
+      <c r="U33" s="47"/>
     </row>
     <row r="34" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C34" s="24">
@@ -75626,15 +75634,15 @@
       <c r="J45" s="40">
         <v>2</v>
       </c>
-      <c r="O45" s="46" t="s">
+      <c r="O45" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="P45" s="46"/>
-      <c r="Q45" s="46"/>
-      <c r="R45" s="46"/>
-      <c r="S45" s="46"/>
-      <c r="T45" s="46"/>
-      <c r="U45" s="46"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="47"/>
+      <c r="R45" s="47"/>
+      <c r="S45" s="47"/>
+      <c r="T45" s="47"/>
+      <c r="U45" s="47"/>
     </row>
     <row r="46" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C46" s="20">

</xml_diff>